<commit_message>
Fixing formulas in calculate deliverables spreadsheet
</commit_message>
<xml_diff>
--- a/Calculate Deliverables.xlsx
+++ b/Calculate Deliverables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\CMSC435-Project-master\CMSC435-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobby\Desktop\CMSC435-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="7965" xr2:uid="{482B6CCF-E02A-4A2A-8DB8-4C4ACE2BABC2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16174" windowHeight="7960" xr2:uid="{482B6CCF-E02A-4A2A-8DB8-4C4ACE2BABC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,15 +438,15 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.59765625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -458,7 +458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -472,7 +472,7 @@
         <v>0.83889999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -486,7 +486,7 @@
         <v>0.2311</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -498,15 +498,15 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -514,56 +514,56 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12">
-        <f>(100*C2)/(C2+B3)</f>
-        <v>14.631401238041644</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <f>(100*C3)/(C3+C2)</f>
+        <v>63.687150837988824</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B13">
-        <f>(100*B2)/(B2+C3)</f>
-        <v>74.806629834254139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <f>(100*B2)/(B2+B3)</f>
+        <v>47.161267850923025</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B14">
-        <f>(100*(C2+B2))/(C2+B2+B3+C3)</f>
-        <v>44.995818232506274</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <f>(100*(C3+B2))/(C3+B3+B2+C2)</f>
+        <v>50.459994424310011</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B15">
-        <f>((C2*B2)-(C3*B3))/SQRT((C2+C3)*(C2+B3)*(B2+C3)*(B2+B3))</f>
-        <v>-0.1321158062505258</v>
+        <f>((C3*B2)-(B3*C2))/SQRT((C3+B3)*(C3+C2)*(B2+B3)*(B2+C2))</f>
+        <v>8.7161408119500808E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I dont even remember what i did here but i think its important so ill commit it
</commit_message>
<xml_diff>
--- a/Calculate Deliverables.xlsx
+++ b/Calculate Deliverables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16174" windowHeight="7960" xr2:uid="{482B6CCF-E02A-4A2A-8DB8-4C4ACE2BABC2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16174" windowHeight="7960" xr2:uid="{482B6CCF-E02A-4A2A-8DB8-4C4ACE2BABC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>true notOne</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>MCC</t>
+  </si>
+  <si>
+    <t>Crystallizable</t>
+  </si>
+  <si>
+    <t>Crystallization failed (inverted)</t>
   </si>
 </sst>
 </file>
@@ -113,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -121,6 +127,16 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA4EEDE-566D-4807-A0B6-049EB8E640A4}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D4"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.59765625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,13 +479,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>2152</v>
+        <v>174</v>
       </c>
       <c r="C2" s="1">
-        <v>783</v>
+        <v>319</v>
       </c>
       <c r="D2" s="2">
-        <v>0.73319999999999996</v>
+        <v>0.35289999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -477,13 +493,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="C3" s="1">
-        <v>421</v>
+        <v>885</v>
       </c>
       <c r="D3" s="2">
-        <v>0.64570000000000005</v>
+        <v>0.77900000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -491,82 +507,145 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>0.90310000000000001</v>
+        <v>0.40939999999999999</v>
       </c>
       <c r="C4" s="2">
-        <v>0.34970000000000001</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12">
+      <c r="C12">
+        <f>(100*B2)/(B2+B3)</f>
+        <v>40.941176470588232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
         <f>(100*C3)/(C3+C2)</f>
-        <v>34.966777408637874</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+        <v>73.504983388704318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <f>(100*(B2+C3))/(B2+C2+C3+B3)</f>
+        <v>65.00920810313076</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="6">
+        <f>((B2*C3)-(C2*B3))/SQRT((B2+C2)*(B2+B3)*(C3+C2)*(C3+B3))</f>
+        <v>0.13808531645175739</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <f>(100*C3)/(C3+C2)</f>
+        <v>73.504983388704318</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="C17">
         <f>(100*B2)/(B2+B3)</f>
-        <v>90.306336550566513</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+        <v>40.941176470588232</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
+      <c r="C18">
         <f>(100*(C3+B2))/(C3+B3+B2+C2)</f>
-        <v>71.731251742403117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+        <v>65.00920810313076</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15">
+      <c r="C19">
         <f>((C3*B2)-(B3*C2))/SQRT((C3+B3)*(C3+C2)*(B2+B3)*(B2+C2))</f>
-        <v>0.3094611746013306</v>
+        <v>0.13808531645175739</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>